<commit_message>
test subsection entfernt und excel tabelle fertig
</commit_message>
<xml_diff>
--- a/swot_analyisis.xlsx
+++ b/swot_analyisis.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FluryD\Documents\LaTeX\git\Strategiepapier-Moschti\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasch\Documents\Strategiepapier-Moschti\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68144582-E9DB-404B-BB80-8B6B9C0F2E81}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6948" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Marktumfeld</t>
   </si>
@@ -47,9 +48,6 @@
     <t>Langfristige Sponsoren</t>
   </si>
   <si>
-    <t>Qualitativ gute Musiker</t>
-  </si>
-  <si>
     <t>Genügend Parkplätze</t>
   </si>
   <si>
@@ -74,9 +72,6 @@
     <t>Stammkunden</t>
   </si>
   <si>
-    <t>Neugierige Konsumenten</t>
-  </si>
-  <si>
     <t>Vergrösserung der Veranstaltungen</t>
   </si>
   <si>
@@ -86,19 +81,70 @@
     <t>Konkurrenzdruck</t>
   </si>
   <si>
-    <t>Zu wenig Kundschaft (z.B. bei Krisen)</t>
-  </si>
-  <si>
     <t>Keine gute, günstige Musiker</t>
   </si>
   <si>
     <t>Welche Stärken treffen auf welche Möglichkeiten?</t>
+  </si>
+  <si>
+    <t>Zu wenig Kundschaft (da abgelegen)</t>
+  </si>
+  <si>
+    <t>zu teure Miete</t>
+  </si>
+  <si>
+    <t>Welche Stärken treffen auf welche Gefahren?</t>
+  </si>
+  <si>
+    <t>Welche Schwächen treffen auf welche Möglichkeiten?</t>
+  </si>
+  <si>
+    <t>Welche Schwächen treffen auf welche Gefahren?</t>
+  </si>
+  <si>
+    <t>Durch Treue Kunden gewinnen wir die Unterstützung des Dorfes</t>
+  </si>
+  <si>
+    <t>Durch die Parkölätze sind auch grössere Evente möglich</t>
+  </si>
+  <si>
+    <t>Neugierige Kunden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Durch gute Musiker kommen neugiereige Kunden </t>
+  </si>
+  <si>
+    <t>Durch das gute Preisleistungsverhältnis bekommt man Stammkunden</t>
+  </si>
+  <si>
+    <t>Durch gute Musiker + Preisleistungsverhältniss mindert sich der Konkurrentdruck</t>
+  </si>
+  <si>
+    <t>Durch treue Kunden können wir die Kosten der Miete begleichen</t>
+  </si>
+  <si>
+    <t>Qualitativ gute Musiker (Jungmusiker)</t>
+  </si>
+  <si>
+    <t>Durch ausgewählte Jungmusiker haben wir geringere Kosten</t>
+  </si>
+  <si>
+    <t>Durch genügend Parkplätze wird die Abgelegenheit kompensiert</t>
+  </si>
+  <si>
+    <t>evt. Umzug in umsatzstärkeres Gebiet</t>
+  </si>
+  <si>
+    <t>Die unglücklichen Nachbaren von der Idee überzeugen -&gt; unterstützen uns</t>
+  </si>
+  <si>
+    <t>Abgelegener Ort ist ideal für grössere Veranstaltungen, bringt dem Dorf Gewinne ein</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -158,14 +204,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -479,154 +525,184 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="38.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C1" s="3" t="s">
+    <row r="1" spans="1:4" ht="38.549999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C4" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C4" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C7" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:4" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="4"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="6"/>
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
       <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
       <c r="B11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="6"/>
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
+      <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="4"/>
-      <c r="B12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
-      <c r="B13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="6"/>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="4"/>
+      <c r="C14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="6"/>
       <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="6"/>
+      <c r="B16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="6"/>
+      <c r="B17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="4"/>
-      <c r="B17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>